<commit_message>
found the getvalue error. needs fixing still
</commit_message>
<xml_diff>
--- a/SubmissionStuff/TCRs_HalfwayHome.xlsx
+++ b/SubmissionStuff/TCRs_HalfwayHome.xlsx
@@ -2703,7 +2703,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="22" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="5" t="s">

</xml_diff>

<commit_message>
Once more, with feeling
</commit_message>
<xml_diff>
--- a/SubmissionStuff/TCRs_HalfwayHome.xlsx
+++ b/SubmissionStuff/TCRs_HalfwayHome.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7434" windowHeight="4488" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7434" windowHeight="4488" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -1857,7 +1857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2702,8 +2702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="7" t="s">

</xml_diff>